<commit_message>
Working on RPM calculation.
</commit_message>
<xml_diff>
--- a/ebaesc_sw/documents/izracuni_bemf_observerja.xlsx
+++ b/ebaesc_sw/documents/izracuni_bemf_observerja.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="26835" windowHeight="13350"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="26835" windowHeight="13350" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Ld</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>dT</t>
+  </si>
+  <si>
+    <t>Kth</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>AD</t>
   </si>
 </sst>
 </file>
@@ -166,6 +175,421 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="sl-SI"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RPM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List2!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List2!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>21333.333333333332</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25263.157894736843</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29090.909090909088</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33103.448275862065</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36923.076923076922</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43636.36363636364</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="58449280"/>
+        <c:axId val="58447744"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="58449280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="58447744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="58447744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="58449280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="sl-SI"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.5678675640405284E-2"/>
+                  <c:y val="7.146877826712339E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List2!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List2!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="56861056"/>
+        <c:axId val="56855168"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="56861056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56855168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="56855168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56861056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafikon 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafikon 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -457,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +950,7 @@
       </c>
       <c r="H2">
         <f>(2*PI()*K2*G2)/60</f>
-        <v>12566.370614359173</v>
+        <v>14660.765716752367</v>
       </c>
       <c r="I2">
         <f>PI()</f>
@@ -536,7 +960,7 @@
         <v>6.2500000000000001E-5</v>
       </c>
       <c r="K2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -567,19 +991,19 @@
         <v>15</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G5">
         <f>F5*0.0000625</f>
-        <v>5.6250000000000007E-4</v>
+        <v>4.3750000000000001E-4</v>
       </c>
       <c r="H5">
         <f>(1/G5)*60</f>
-        <v>106666.66666666666</v>
+        <v>137142.85714285716</v>
       </c>
       <c r="I5">
         <f>H5/K2</f>
-        <v>17777.777777777777</v>
+        <v>19591.836734693879</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -615,7 +1039,7 @@
       </c>
       <c r="C9" s="3">
         <f>((B2*J2)/(A2+(J2*C2)))*H2</f>
-        <v>0.4358278825789309</v>
+        <v>0.50846586300875263</v>
       </c>
       <c r="D9" s="3">
         <f>A2/(A2+(J2*C2))</f>
@@ -657,15 +1081,15 @@
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>A12*(L2/H2)</f>
-        <v>3.1999999999999994E-2</v>
+        <v>2.7428571428571431E-2</v>
       </c>
       <c r="B15">
         <f>B12*(L2/H2)</f>
-        <v>5.026548245743669</v>
+        <v>4.3084699249231448</v>
       </c>
       <c r="C15">
         <f>(J2*H2)/I2</f>
-        <v>0.25000000000000006</v>
+        <v>0.29166666666666663</v>
       </c>
     </row>
   </sheetData>
@@ -676,13 +1100,136 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.6</v>
+      </c>
+      <c r="B2">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <f>(1/(B2*0.0000625))*60</f>
+        <v>21333.333333333332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.7</v>
+      </c>
+      <c r="B3">
+        <v>38</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C8" si="0">(1/(B3*0.0000625))*60</f>
+        <v>25263.157894736843</v>
+      </c>
+      <c r="D3">
+        <f>C3-C2</f>
+        <v>3929.8245614035113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.8</v>
+      </c>
+      <c r="B4">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>29090.909090909088</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D8" si="1">C4-C3</f>
+        <v>3827.7511961722448</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.9</v>
+      </c>
+      <c r="B5">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>33103.448275862065</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>4012.5391849529769</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>36923.076923076922</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>3819.6286472148568</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B7">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>40000</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>3076.923076923078</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1.2</v>
+      </c>
+      <c r="B8">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>43636.36363636364</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>3636.3636363636397</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Flashing has problems. Improved startup var calculation.
</commit_message>
<xml_diff>
--- a/ebaesc_sw/documents/izracuni_bemf_observerja.xlsx
+++ b/ebaesc_sw/documents/izracuni_bemf_observerja.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="26835" windowHeight="13350" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="26835" windowHeight="13350"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -306,11 +306,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="58449280"/>
-        <c:axId val="58447744"/>
+        <c:axId val="120054144"/>
+        <c:axId val="120055680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58449280"/>
+        <c:axId val="120054144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -320,12 +320,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58447744"/>
+        <c:crossAx val="120055680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58447744"/>
+        <c:axId val="120055680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -336,7 +336,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58449280"/>
+        <c:crossAx val="120054144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -484,11 +484,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="56861056"/>
-        <c:axId val="56855168"/>
+        <c:axId val="121268864"/>
+        <c:axId val="121274752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56861056"/>
+        <c:axId val="121268864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -498,12 +498,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56855168"/>
+        <c:crossAx val="121274752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56855168"/>
+        <c:axId val="121274752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -514,7 +514,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56861056"/>
+        <c:crossAx val="121268864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -890,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,18 +955,18 @@
         <v>42.619148899999999</v>
       </c>
       <c r="G2">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="H2">
         <f>(2*PI()*K2*G2)/60</f>
-        <v>14660.765716752367</v>
+        <v>43982.297150257109</v>
       </c>
       <c r="I2">
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
       <c r="J2" s="1">
-        <v>6.2500000000000001E-5</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K2">
         <v>7</v>
@@ -1002,17 +1002,17 @@
       <c r="F5">
         <v>7</v>
       </c>
-      <c r="G5">
-        <f>F5*0.0000625</f>
-        <v>4.3750000000000001E-4</v>
+      <c r="G5" s="1">
+        <f>F5*J2</f>
+        <v>3.5E-4</v>
       </c>
       <c r="H5">
         <f>(1/G5)*60</f>
-        <v>137142.85714285716</v>
+        <v>171428.57142857145</v>
       </c>
       <c r="I5">
         <f>H5/K2</f>
-        <v>19591.836734693879</v>
+        <v>24489.795918367348</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1040,19 +1040,19 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f>(J2/(A2+(J2*C2)))*(D2/E2)</f>
-        <v>0.74652564196882121</v>
+        <v>0.65557835563759426</v>
       </c>
       <c r="B9" s="3">
         <f>(J2/(A2+(J2*C2)))*(F2/E2)</f>
-        <v>0.74652564196882121</v>
+        <v>0.65557835563759426</v>
       </c>
       <c r="C9" s="3">
         <f>((B2*J2)/(A2+(J2*C2)))*H2</f>
-        <v>0.50846586300875263</v>
+        <v>1.3395623497540237</v>
       </c>
       <c r="D9" s="3">
         <f>A2/(A2+(J2*C2))</f>
-        <v>0.55491329479768792</v>
+        <v>0.60913705583756339</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1090,15 +1090,15 @@
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>A12*(L2/H2)</f>
-        <v>2.7428571428571431E-2</v>
+        <v>9.1428571428571418E-3</v>
       </c>
       <c r="B15">
         <f>B12*(L2/H2)</f>
-        <v>4.3084699249231448</v>
+        <v>1.4361566416410483</v>
       </c>
       <c r="C15">
         <f>(J2*H2)/I2</f>
-        <v>0.29166666666666663</v>
+        <v>0.70000000000000018</v>
       </c>
     </row>
   </sheetData>
@@ -1111,7 +1111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update, parameters optimized for emax motor (start current, start ramp, min. speed).
</commit_message>
<xml_diff>
--- a/ebaesc_sw/documents/izracuni_bemf_observerja.xlsx
+++ b/ebaesc_sw/documents/izracuni_bemf_observerja.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="26835" windowHeight="13350"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="26835" windowHeight="13290"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -232,7 +231,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -306,11 +304,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="120054144"/>
-        <c:axId val="120055680"/>
+        <c:axId val="63548032"/>
+        <c:axId val="88740224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120054144"/>
+        <c:axId val="63548032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -320,12 +318,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120055680"/>
+        <c:crossAx val="88740224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="120055680"/>
+        <c:axId val="88740224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -336,14 +334,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120054144"/>
+        <c:crossAx val="63548032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -373,7 +370,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -484,11 +480,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121268864"/>
-        <c:axId val="121274752"/>
+        <c:axId val="88761472"/>
+        <c:axId val="88763008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121268864"/>
+        <c:axId val="88761472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -498,12 +494,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121274752"/>
+        <c:crossAx val="88763008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121274752"/>
+        <c:axId val="88763008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -514,14 +510,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121268864"/>
+        <c:crossAx val="88761472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -891,7 +886,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,13 +931,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>6.0000000000000002E-6</v>
+        <v>1.5999999999999999E-6</v>
       </c>
       <c r="B2" s="1">
-        <v>6.0000000000000002E-6</v>
+        <v>1.5999999999999999E-6</v>
       </c>
       <c r="C2" s="1">
-        <v>7.6999999999999999E-2</v>
+        <v>1.95E-2</v>
       </c>
       <c r="D2" s="1">
         <v>42.619148899999999</v>
@@ -1040,19 +1035,19 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f>(J2/(A2+(J2*C2)))*(D2/E2)</f>
-        <v>0.65557835563759426</v>
+        <v>2.5077463312739043</v>
       </c>
       <c r="B9" s="3">
         <f>(J2/(A2+(J2*C2)))*(F2/E2)</f>
-        <v>0.65557835563759426</v>
+        <v>2.5077463312739043</v>
       </c>
       <c r="C9" s="3">
         <f>((B2*J2)/(A2+(J2*C2)))*H2</f>
-        <v>1.3395623497540237</v>
+        <v>1.3664402998138132</v>
       </c>
       <c r="D9" s="3">
         <f>A2/(A2+(J2*C2))</f>
-        <v>0.60913705583756339</v>
+        <v>0.62135922330097082</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updating system state machine, cleanup, EEPROM store update.
</commit_message>
<xml_diff>
--- a/ebaesc_sw/documents/izracuni_bemf_observerja.xlsx
+++ b/ebaesc_sw/documents/izracuni_bemf_observerja.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Ld</t>
   </si>
@@ -60,12 +60,6 @@
     <t>TO</t>
   </si>
   <si>
-    <t>TO_att</t>
-  </si>
-  <si>
-    <t>TO_f0</t>
-  </si>
-  <si>
     <t>TO_Kp</t>
   </si>
   <si>
@@ -121,6 +115,50 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <r>
+      <t>TO_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>ω</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TO_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>ξ</t>
+    </r>
+  </si>
+  <si>
+    <t>BEMF_DQ</t>
   </si>
 </sst>
 </file>
@@ -130,7 +168,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,16 +184,36 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -163,15 +221,112 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Navadno" xfId="0" builtinId="0"/>
@@ -304,11 +459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="63548032"/>
-        <c:axId val="88740224"/>
+        <c:axId val="61616512"/>
+        <c:axId val="61618048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63548032"/>
+        <c:axId val="61616512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -318,12 +473,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88740224"/>
+        <c:crossAx val="61618048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88740224"/>
+        <c:axId val="61618048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -334,7 +489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63548032"/>
+        <c:crossAx val="61616512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -480,11 +635,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="88761472"/>
-        <c:axId val="88763008"/>
+        <c:axId val="61651584"/>
+        <c:axId val="61657472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88761472"/>
+        <c:axId val="61651584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,12 +649,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88763008"/>
+        <c:crossAx val="61657472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88763008"/>
+        <c:axId val="61657472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,7 +665,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88761472"/>
+        <c:crossAx val="61651584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -886,7 +1041,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,187 +1068,213 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>24</v>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1.5999999999999999E-6</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1.5999999999999999E-6</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.95E-2</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="A2" s="2">
+        <v>2.3E-3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2.3E-3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="D2" s="2">
         <v>42.619148899999999</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>330</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
         <f>D2</f>
         <v>42.619148899999999</v>
       </c>
-      <c r="G2">
-        <v>60000</v>
-      </c>
-      <c r="H2">
+      <c r="G2" s="3">
+        <v>20000</v>
+      </c>
+      <c r="H2" s="4">
         <f>(2*PI()*K2*G2)/60</f>
-        <v>43982.297150257109</v>
-      </c>
-      <c r="I2">
+        <v>14660.765716752367</v>
+      </c>
+      <c r="I2" s="4">
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="2">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="3">
         <v>7</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
+      <c r="A4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
       <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5">
+    </row>
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="F5" s="3">
         <v>7</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="5">
         <f>F5*J2</f>
         <v>3.5E-4</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <f>(1/G5)*60</f>
         <v>171428.57142857145</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="4">
         <f>H5/K2</f>
         <v>24489.795918367348</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0.8</v>
-      </c>
-      <c r="B6">
+      <c r="A6" s="12">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13">
         <v>40</v>
       </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="14">
         <f>(J2/(A2+(J2*C2)))*(D2/E2)</f>
-        <v>2.5077463312739043</v>
-      </c>
-      <c r="B9" s="3">
+        <v>2.8063654076620178E-3</v>
+      </c>
+      <c r="B9" s="15">
         <f>(J2/(A2+(J2*C2)))*(F2/E2)</f>
-        <v>2.5077463312739043</v>
-      </c>
-      <c r="C9" s="3">
+        <v>2.8063654076620178E-3</v>
+      </c>
+      <c r="C9" s="15">
         <f>((B2*J2)/(A2+(J2*C2)))*H2</f>
-        <v>1.3664402998138132</v>
-      </c>
-      <c r="D9" s="3">
+        <v>0.7327197120497706</v>
+      </c>
+      <c r="D9" s="16">
         <f>A2/(A2+(J2*C2))</f>
-        <v>0.62135922330097082</v>
-      </c>
+        <v>0.9995654063450673</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f>2*A6*2*PI()*B6</f>
-        <v>402.12385965949352</v>
-      </c>
-      <c r="B12">
-        <f>(2*PI()*B6)^2</f>
-        <v>63165.468166971892</v>
-      </c>
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17">
+        <f>(2*A6*2*PI()*B6*A2)-C2</f>
+        <v>1.1361060965210439</v>
+      </c>
+      <c r="B12" s="18">
+        <f>((2*PI()*B6)^2)*A2</f>
+        <v>145.28057678403536</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="4">
         <f>A12*(L2/H2)</f>
-        <v>9.1428571428571418E-3</v>
-      </c>
-      <c r="B15">
+        <v>7.7492957630640905E-5</v>
+      </c>
+      <c r="B15" s="4">
         <f>B12*(L2/H2)</f>
-        <v>1.4361566416410483</v>
-      </c>
-      <c r="C15">
+        <v>9.9094808273232343E-3</v>
+      </c>
+      <c r="C15" s="4">
         <f>(J2*H2)/I2</f>
-        <v>0.70000000000000018</v>
+        <v>0.23333333333333331</v>
       </c>
     </row>
   </sheetData>
@@ -1114,22 +1295,22 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>32</v>
-      </c>
-      <c r="I1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>